<commit_message>
Programul pentru introducere - citire de valori si afisare folosind consola, diferitele tipuri de date, operatii pe numere si ordinea lor, operatii pe stringuri, declarare si initializare a variabilelor, convertirea unui tip de date in altul, operatii booleene si structura if..else
</commit_message>
<xml_diff>
--- a/AlgoritmiSiStructuriDeDate1/Prezenta.xlsx
+++ b/AlgoritmiSiStructuriDeDate1/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Geoinformatica_Promotia_2025_2028\AlgoritmiSiStructuriDeDate1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08256057-A974-4DDC-94B6-A34E8FCD7529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B4FCC5-8CAB-4EB2-8E28-CCB09DDD34D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Prenume Nume</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Claudiu Druța</t>
   </si>
   <si>
-    <t>Daniela Cionca (Maria)</t>
-  </si>
-  <si>
     <t>Sorin Fechete</t>
   </si>
   <si>
@@ -109,6 +106,36 @@
   </si>
   <si>
     <t>Amanda Hajdu</t>
+  </si>
+  <si>
+    <t>Silvia Naghi</t>
+  </si>
+  <si>
+    <t>Raul Andrei</t>
+  </si>
+  <si>
+    <t>Levente Nagy</t>
+  </si>
+  <si>
+    <t>Mark Pop</t>
+  </si>
+  <si>
+    <t>Alessandro Vereș-Pop</t>
+  </si>
+  <si>
+    <t>Daniela Cionca (Mărie)</t>
+  </si>
+  <si>
+    <t>Luca Șeicaru</t>
+  </si>
+  <si>
+    <t>Attila Bunta</t>
+  </si>
+  <si>
+    <t>Codruț Avram</t>
+  </si>
+  <si>
+    <t>Victor Lazăr</t>
   </si>
 </sst>
 </file>
@@ -652,7 +679,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -722,10 +749,10 @@
     </row>
     <row r="3" spans="2:19">
       <c r="B3" s="4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -742,14 +769,14 @@
       <c r="P3" s="7"/>
       <c r="Q3" s="8">
         <f>SUM(C3:P3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C4" s="9">
         <v>1</v>
@@ -764,7 +791,7 @@
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
@@ -779,7 +806,7 @@
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C6" s="9">
         <v>1</v>
@@ -794,22 +821,22 @@
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C7" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7" s="9"/>
       <c r="S7" s="10"/>
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C8" s="9">
         <v>1</v>
@@ -824,37 +851,37 @@
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C9" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9" s="9"/>
       <c r="S9" s="10"/>
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C10" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10" s="9"/>
       <c r="S10" s="10"/>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
@@ -869,114 +896,150 @@
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12" s="9"/>
       <c r="S12" s="10"/>
     </row>
     <row r="13" spans="2:19">
-      <c r="B13" s="4"/>
-      <c r="C13" s="9"/>
+      <c r="B13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" s="9"/>
       <c r="S13" s="10"/>
     </row>
     <row r="14" spans="2:19">
-      <c r="B14" s="4"/>
-      <c r="C14" s="9"/>
+      <c r="B14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="9">
+        <v>2</v>
+      </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R14" s="9"/>
       <c r="S14" s="10"/>
     </row>
     <row r="15" spans="2:19">
-      <c r="B15" s="4"/>
-      <c r="C15" s="9"/>
+      <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="9">
+        <v>2</v>
+      </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R15" s="9"/>
       <c r="S15" s="10"/>
     </row>
     <row r="16" spans="2:19">
-      <c r="B16" s="4"/>
-      <c r="C16" s="9"/>
+      <c r="B16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="9">
+        <v>2</v>
+      </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R16" s="9"/>
       <c r="S16" s="10"/>
     </row>
     <row r="17" spans="2:19">
-      <c r="B17" s="4"/>
-      <c r="C17" s="9"/>
+      <c r="B17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1</v>
+      </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="9"/>
       <c r="S17" s="10"/>
     </row>
     <row r="18" spans="2:19">
-      <c r="B18" s="4"/>
-      <c r="C18" s="9"/>
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="9">
+        <v>2</v>
+      </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R18" s="9"/>
       <c r="S18" s="10"/>
     </row>
     <row r="19" spans="2:19">
-      <c r="B19" s="4"/>
-      <c r="C19" s="9"/>
+      <c r="B19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="9">
+        <v>2</v>
+      </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R19" s="9"/>
       <c r="S19" s="10"/>
     </row>
     <row r="20" spans="2:19">
-      <c r="B20" s="4"/>
-      <c r="C20" s="9"/>
+      <c r="B20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="9">
+        <v>1</v>
+      </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R20" s="9"/>
       <c r="S20" s="10"/>
     </row>
     <row r="21" spans="2:19">
-      <c r="B21" s="4"/>
-      <c r="C21" s="9"/>
+      <c r="B21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21" s="9"/>
       <c r="S21" s="10"/>

</xml_diff>